<commit_message>
zero indexed spawn tiles continue gs attack roll
</commit_message>
<xml_diff>
--- a/location_cards.xlsx
+++ b/location_cards.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8cb4a1cf07ac5584/Python/Pyxel projects/SpaceMarine_DeathAngel_GAME/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="328" documentId="8_{F76DA7B4-882A-43E1-8759-B2A2BF66176B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC63EEB5-9492-4689-8409-524CAE7D1145}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{84DFED77-1B01-4041-8544-38DF0EC5AF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6940121-2F69-422B-A33B-BEBFDDA68415}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="2685" windowWidth="29760" windowHeight="15435" xr2:uid="{A31C0A8A-4D9A-4B27-91FD-BDF525427EA4}"/>
+    <workbookView xWindow="3828" yWindow="2784" windowWidth="17280" windowHeight="8880" xr2:uid="{A31C0A8A-4D9A-4B27-91FD-BDF525427EA4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="location_cards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -186,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +196,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,16 +239,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -255,9 +270,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -295,7 +310,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -401,7 +416,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -543,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -553,69 +568,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE8C19C-CFB9-4C1D-90CE-D11C1101D331}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="174.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="174.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
@@ -625,13 +640,13 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -643,7 +658,7 @@
         <v>5</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K2">
         <v>6</v>
@@ -661,8 +676,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
@@ -672,7 +687,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -684,13 +699,13 @@
         <v>4</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
         <v>5</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>6</v>
@@ -708,8 +723,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
@@ -719,25 +734,25 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I4" t="s">
         <v>5</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K4">
         <v>7</v>
@@ -755,8 +770,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -766,25 +781,25 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K5">
         <v>5</v>
@@ -802,8 +817,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
@@ -813,25 +828,25 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6" t="s">
         <v>2</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K6">
         <v>5</v>
@@ -849,8 +864,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
@@ -860,19 +875,19 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7" t="s">
         <v>4</v>
@@ -896,8 +911,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
@@ -907,25 +922,25 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I8" t="s">
         <v>2</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -943,8 +958,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
@@ -954,25 +969,25 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I9" t="s">
         <v>5</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K9">
         <v>6</v>
@@ -990,8 +1005,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
@@ -1001,25 +1016,25 @@
         <v>5</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
       <c r="G10" t="s">
         <v>6</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I10" t="s">
         <v>4</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K10">
         <v>7</v>

</xml_diff>